<commit_message>
Add detailed output CSV files for thermal, wind, and hydro units; initialize BESS charging and discharging summaries; implement total boundary data input function
- Created output CSV files for thermal units, wind units, and their respective wasted outputs.
- Added detailed hydro output CSV files for multiple intervals.
- Initialized summary CSV files for BESS charging, discharging, and forced load curtailment with zero values.
- Implemented the `_get_totalboundarydata.jl` function to load and process input data for generators, branches, loads, and storage units, including hydro data.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanyiping/Documents/GitHub/module_unitcommitment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAF8FE9-0D44-F646-80B7-16AE6F250B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C7959-9A31-3247-A5A2-ED4CCD76CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="22960" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1460" windowWidth="38400" windowHeight="21100" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units_frequencyparam" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,28 @@
     <sheet name="load_curve" sheetId="7" r:id="rId7"/>
     <sheet name="load_data" sheetId="8" r:id="rId8"/>
     <sheet name="data_centra" sheetId="9" r:id="rId9"/>
+    <sheet name="hydro_data" sheetId="10" r:id="rId10"/>
+    <sheet name="hydro_seasoncurve" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>index</t>
   </si>
@@ -204,6 +219,15 @@
   </si>
   <si>
     <t>Gens_t1</t>
+  </si>
+  <si>
+    <t>qmax</t>
+  </si>
+  <si>
+    <t>q0</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -290,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -319,11 +343,32 @@
     <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -368,6 +413,17 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fg(0.15,0.4)"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tg(6,14)"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Rg(0.04,0.1)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{90DA1D3D-F6FB-2945-BBFB-035702378813}" name="表11_10" displayName="表11_10" ref="A1:B169" totalsRowShown="0">
+  <autoFilter ref="A1:B169" xr:uid="{90DA1D3D-F6FB-2945-BBFB-035702378813}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CFC9E3BB-3CBD-2B49-987D-49950F1CF078}" name="index"/>
+    <tableColumn id="2" xr3:uid="{5CFC1256-5DCA-0343-804E-77C92C9A264A}" name="p"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -426,7 +482,7 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Gens_x0"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Gens_t0"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="Gens_p0"/>
-    <tableColumn id="14" xr3:uid="{EF870B2E-34C2-234E-BE9A-84EC291628D6}" name="Gens_t1" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{EF870B2E-34C2-234E-BE9A-84EC291628D6}" name="Gens_t1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -483,6 +539,21 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A802B22F-A946-6145-BB93-E071DBF84974}" name="Table10" displayName="Table10" ref="A1:F9" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F9" xr:uid="{A802B22F-A946-6145-BB93-E071DBF84974}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2C34CE5F-8262-7546-9A26-C746718FA026}" name="index"/>
+    <tableColumn id="2" xr3:uid="{1FC8BCD2-C02B-C740-BBC8-19CD824FD767}" name="locatebus"/>
+    <tableColumn id="3" xr3:uid="{8041F6BD-D058-4640-B99B-739BF9B6FA31}" name="p_max"/>
+    <tableColumn id="4" xr3:uid="{DEA14585-2788-FB43-9A3D-C768216ECB72}" name="p_min"/>
+    <tableColumn id="5" xr3:uid="{48E370AE-D3AF-E64F-8116-3DD9FA90D2B9}" name="qmax"/>
+    <tableColumn id="6" xr3:uid="{F43521CB-B297-864B-9BC3-CB246032D773}" name="q0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -890,6 +961,1588 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA492298-718A-294F-AA8A-B9EF8645097E}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FDC3B1-AAE8-EB49-94CD-DAD9D4E18BE9}">
+  <dimension ref="A1:N169"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2.4110899999999997</v>
+      </c>
+      <c r="N26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="7">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="9">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="7">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="7">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="7">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="8">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="8">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="7">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="7">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="8">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="8">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="9">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="8">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="8">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="7">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="8">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="7">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="8">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="7">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="8">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="7">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="8">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="7">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="8">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="7">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="8">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="7">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="8">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="7">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="8">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="7">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="8">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="7">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113" s="8">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114" s="9">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115" s="8">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" s="7">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117" s="8">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118" s="7">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119" s="8">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120" s="7">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121" s="8">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122" s="7">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123" s="8">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124" s="7">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125" s="8">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126" s="7">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127" s="8">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128" s="7">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129" s="8">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130" s="7">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131" s="8">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132" s="7">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133" s="8">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134" s="7">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135" s="8">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136" s="7">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137" s="8">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138" s="9">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139" s="8">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140" s="7">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141" s="8">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>141</v>
+      </c>
+      <c r="B142" s="7">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>142</v>
+      </c>
+      <c r="B143" s="8">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>143</v>
+      </c>
+      <c r="B144" s="7">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>144</v>
+      </c>
+      <c r="B145" s="8">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146" s="7">
+        <v>2.4110899999999997</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>146</v>
+      </c>
+      <c r="B147" s="8">
+        <v>2.5888499999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>147</v>
+      </c>
+      <c r="B148" s="7">
+        <v>2.5813699999999997</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>148</v>
+      </c>
+      <c r="B149" s="8">
+        <v>2.6040299999999998</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>149</v>
+      </c>
+      <c r="B150" s="7">
+        <v>2.6296599999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>150</v>
+      </c>
+      <c r="B151" s="8">
+        <v>2.6892799999999997</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>151</v>
+      </c>
+      <c r="B152" s="7">
+        <v>3.0072899999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>152</v>
+      </c>
+      <c r="B153" s="8">
+        <v>3.1943999999999995</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>153</v>
+      </c>
+      <c r="B154" s="7">
+        <v>3.1191599999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>154</v>
+      </c>
+      <c r="B155" s="8">
+        <v>3.0931999999999995</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>155</v>
+      </c>
+      <c r="B156" s="7">
+        <v>3.6147100000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>156</v>
+      </c>
+      <c r="B157" s="8">
+        <v>3.6091000000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>157</v>
+      </c>
+      <c r="B158" s="7">
+        <v>3.5879799999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>158</v>
+      </c>
+      <c r="B159" s="8">
+        <v>3.5596000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>159</v>
+      </c>
+      <c r="B160" s="7">
+        <v>3.5954600000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>160</v>
+      </c>
+      <c r="B161" s="8">
+        <v>3.1656900000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>161</v>
+      </c>
+      <c r="B162" s="9">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>162</v>
+      </c>
+      <c r="B163" s="8">
+        <v>2.71414</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>163</v>
+      </c>
+      <c r="B164" s="7">
+        <v>2.8156699999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>164</v>
+      </c>
+      <c r="B165" s="8">
+        <v>2.6108499999999997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>165</v>
+      </c>
+      <c r="B166" s="7">
+        <v>2.6764099999999997</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>166</v>
+      </c>
+      <c r="B167" s="8">
+        <v>3.1145399999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>167</v>
+      </c>
+      <c r="B168" s="7">
+        <v>3.11355</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>168</v>
+      </c>
+      <c r="B169" s="8">
+        <v>2.7362499999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -1593,8 +3246,8 @@
   </sheetPr>
   <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3041,7 +4694,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3316,5 +4969,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>